<commit_message>
remove Node Tech Compete from biodiesel and ethanol steam competitions
</commit_message>
<xml_diff>
--- a/csv/model/sector_biodiesel/formula_sector_biodiesel_AB.xlsx
+++ b/csv/model/sector_biodiesel/formula_sector_biodiesel_AB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Brad_Griffin\CIMS\cims-models\csv\model\sector_biodiesel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\sector_biodiesel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63D65652-BC68-40D6-850D-836A833A98FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCE2D774-B0BC-447D-8421-63E05FD5E033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{35C42C4C-BD1E-448D-97FE-9337F5DB5CB5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9599A1CF-F3E2-4AF8-BDF0-43FE76B776EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="101">
   <si>
     <t>CIMS.CAN.AB.Biodiesel.Steam</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>Steam</t>
-  </si>
-  <si>
-    <t>Node Tech Compete</t>
   </si>
   <si>
     <t>Electric</t>
@@ -48950,7 +48947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532C0A2F-EBF6-40CF-B92B-5657805EC291}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF8B7EA-2BC6-40F2-9CA1-6BD744D3C201}">
   <dimension ref="A1:X204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -53475,7 +53472,7 @@
         <v>20</v>
       </c>
       <c r="H78" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
@@ -53624,7 +53621,7 @@
         <v>78</v>
       </c>
       <c r="F81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G81" t="s">
         <v>7</v>
@@ -53647,7 +53644,7 @@
         <v>78</v>
       </c>
       <c r="F82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G82" t="s">
         <v>62</v>
@@ -53716,7 +53713,7 @@
         <v>78</v>
       </c>
       <c r="F83" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G83" t="s">
         <v>64</v>
@@ -53785,7 +53782,7 @@
         <v>78</v>
       </c>
       <c r="F84" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G84" t="s">
         <v>65</v>
@@ -53854,7 +53851,7 @@
         <v>78</v>
       </c>
       <c r="F85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G85" t="s">
         <v>67</v>
@@ -53883,7 +53880,7 @@
         <v>78</v>
       </c>
       <c r="F86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G86" t="s">
         <v>68</v>
@@ -53952,7 +53949,7 @@
         <v>78</v>
       </c>
       <c r="F87" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G87" t="s">
         <v>69</v>
@@ -54021,7 +54018,7 @@
         <v>78</v>
       </c>
       <c r="F88" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G88" t="s">
         <v>71</v>
@@ -54090,7 +54087,7 @@
         <v>78</v>
       </c>
       <c r="F89" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G89" t="s">
         <v>54</v>
@@ -54162,7 +54159,7 @@
         <v>78</v>
       </c>
       <c r="F90" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G90" t="s">
         <v>7</v>
@@ -54185,7 +54182,7 @@
         <v>78</v>
       </c>
       <c r="F91" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G91" t="s">
         <v>62</v>
@@ -54254,7 +54251,7 @@
         <v>78</v>
       </c>
       <c r="F92" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G92" t="s">
         <v>64</v>
@@ -54323,7 +54320,7 @@
         <v>78</v>
       </c>
       <c r="F93" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G93" t="s">
         <v>65</v>
@@ -54392,7 +54389,7 @@
         <v>78</v>
       </c>
       <c r="F94" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G94" t="s">
         <v>67</v>
@@ -54421,7 +54418,7 @@
         <v>78</v>
       </c>
       <c r="F95" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G95" t="s">
         <v>68</v>
@@ -54490,7 +54487,7 @@
         <v>78</v>
       </c>
       <c r="F96" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G96" t="s">
         <v>69</v>
@@ -54559,7 +54556,7 @@
         <v>78</v>
       </c>
       <c r="F97" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G97" t="s">
         <v>71</v>
@@ -54628,7 +54625,7 @@
         <v>78</v>
       </c>
       <c r="F98" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G98" t="s">
         <v>54</v>
@@ -54700,7 +54697,7 @@
         <v>78</v>
       </c>
       <c r="F99" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G99" t="s">
         <v>7</v>
@@ -54723,7 +54720,7 @@
         <v>78</v>
       </c>
       <c r="F100" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G100" t="s">
         <v>62</v>
@@ -54792,7 +54789,7 @@
         <v>78</v>
       </c>
       <c r="F101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G101" t="s">
         <v>64</v>
@@ -54861,7 +54858,7 @@
         <v>78</v>
       </c>
       <c r="F102" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G102" t="s">
         <v>65</v>
@@ -54930,7 +54927,7 @@
         <v>78</v>
       </c>
       <c r="F103" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G103" t="s">
         <v>67</v>
@@ -54959,7 +54956,7 @@
         <v>78</v>
       </c>
       <c r="F104" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G104" t="s">
         <v>68</v>
@@ -55028,7 +55025,7 @@
         <v>78</v>
       </c>
       <c r="F105" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G105" t="s">
         <v>69</v>
@@ -55097,7 +55094,7 @@
         <v>78</v>
       </c>
       <c r="F106" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G106" t="s">
         <v>71</v>
@@ -55166,7 +55163,7 @@
         <v>78</v>
       </c>
       <c r="F107" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G107" t="s">
         <v>54</v>
@@ -55238,7 +55235,7 @@
         <v>78</v>
       </c>
       <c r="F108" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G108" t="s">
         <v>7</v>
@@ -55261,7 +55258,7 @@
         <v>78</v>
       </c>
       <c r="F109" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G109" t="s">
         <v>62</v>
@@ -55330,7 +55327,7 @@
         <v>78</v>
       </c>
       <c r="F110" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G110" t="s">
         <v>64</v>
@@ -55399,7 +55396,7 @@
         <v>78</v>
       </c>
       <c r="F111" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G111" t="s">
         <v>65</v>
@@ -55468,7 +55465,7 @@
         <v>78</v>
       </c>
       <c r="F112" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G112" t="s">
         <v>67</v>
@@ -55497,7 +55494,7 @@
         <v>78</v>
       </c>
       <c r="F113" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G113" t="s">
         <v>68</v>
@@ -55566,7 +55563,7 @@
         <v>78</v>
       </c>
       <c r="F114" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G114" t="s">
         <v>69</v>
@@ -55635,7 +55632,7 @@
         <v>78</v>
       </c>
       <c r="F115" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G115" t="s">
         <v>71</v>
@@ -55704,7 +55701,7 @@
         <v>78</v>
       </c>
       <c r="F116" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G116" t="s">
         <v>54</v>
@@ -55776,7 +55773,7 @@
         <v>78</v>
       </c>
       <c r="F117" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G117" t="s">
         <v>54</v>
@@ -55848,13 +55845,13 @@
         <v>78</v>
       </c>
       <c r="F118" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G118" t="s">
         <v>54</v>
       </c>
       <c r="J118" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L118" t="s">
         <v>70</v>
@@ -55920,7 +55917,7 @@
         <v>78</v>
       </c>
       <c r="F119" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G119" t="s">
         <v>7</v>
@@ -55943,7 +55940,7 @@
         <v>78</v>
       </c>
       <c r="F120" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G120" t="s">
         <v>62</v>
@@ -56012,7 +56009,7 @@
         <v>78</v>
       </c>
       <c r="F121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G121" t="s">
         <v>64</v>
@@ -56081,7 +56078,7 @@
         <v>78</v>
       </c>
       <c r="F122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G122" t="s">
         <v>65</v>
@@ -56150,7 +56147,7 @@
         <v>78</v>
       </c>
       <c r="F123" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G123" t="s">
         <v>67</v>
@@ -56179,7 +56176,7 @@
         <v>78</v>
       </c>
       <c r="F124" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G124" t="s">
         <v>68</v>
@@ -56248,7 +56245,7 @@
         <v>78</v>
       </c>
       <c r="F125" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G125" t="s">
         <v>69</v>
@@ -56317,7 +56314,7 @@
         <v>78</v>
       </c>
       <c r="F126" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G126" t="s">
         <v>71</v>
@@ -56386,7 +56383,7 @@
         <v>78</v>
       </c>
       <c r="F127" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G127" t="s">
         <v>54</v>
@@ -56458,7 +56455,7 @@
         <v>78</v>
       </c>
       <c r="F128" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G128" t="s">
         <v>54</v>
@@ -56530,13 +56527,13 @@
         <v>78</v>
       </c>
       <c r="F129" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G129" t="s">
         <v>54</v>
       </c>
       <c r="J129" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L129" t="s">
         <v>70</v>
@@ -56602,7 +56599,7 @@
         <v>78</v>
       </c>
       <c r="F130" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G130" t="s">
         <v>7</v>
@@ -56625,7 +56622,7 @@
         <v>78</v>
       </c>
       <c r="F131" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G131" t="s">
         <v>62</v>
@@ -56694,7 +56691,7 @@
         <v>78</v>
       </c>
       <c r="F132" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G132" t="s">
         <v>64</v>
@@ -56763,7 +56760,7 @@
         <v>78</v>
       </c>
       <c r="F133" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G133" t="s">
         <v>65</v>
@@ -56832,7 +56829,7 @@
         <v>78</v>
       </c>
       <c r="F134" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G134" t="s">
         <v>67</v>
@@ -56861,7 +56858,7 @@
         <v>78</v>
       </c>
       <c r="F135" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G135" t="s">
         <v>68</v>
@@ -56930,7 +56927,7 @@
         <v>78</v>
       </c>
       <c r="F136" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G136" t="s">
         <v>69</v>
@@ -56999,7 +56996,7 @@
         <v>78</v>
       </c>
       <c r="F137" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G137" t="s">
         <v>71</v>
@@ -57068,7 +57065,7 @@
         <v>78</v>
       </c>
       <c r="F138" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G138" t="s">
         <v>54</v>
@@ -57140,7 +57137,7 @@
         <v>78</v>
       </c>
       <c r="F139" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G139" t="s">
         <v>54</v>
@@ -57212,7 +57209,7 @@
         <v>78</v>
       </c>
       <c r="F140" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G140" t="s">
         <v>7</v>
@@ -57235,7 +57232,7 @@
         <v>78</v>
       </c>
       <c r="F141" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G141" t="s">
         <v>62</v>
@@ -57304,7 +57301,7 @@
         <v>78</v>
       </c>
       <c r="F142" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G142" t="s">
         <v>64</v>
@@ -57373,7 +57370,7 @@
         <v>78</v>
       </c>
       <c r="F143" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G143" t="s">
         <v>65</v>
@@ -57442,7 +57439,7 @@
         <v>78</v>
       </c>
       <c r="F144" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G144" t="s">
         <v>67</v>
@@ -57471,7 +57468,7 @@
         <v>78</v>
       </c>
       <c r="F145" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G145" t="s">
         <v>68</v>
@@ -57540,7 +57537,7 @@
         <v>78</v>
       </c>
       <c r="F146" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G146" t="s">
         <v>69</v>
@@ -57609,7 +57606,7 @@
         <v>78</v>
       </c>
       <c r="F147" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G147" t="s">
         <v>71</v>
@@ -57678,7 +57675,7 @@
         <v>78</v>
       </c>
       <c r="F148" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G148" t="s">
         <v>54</v>
@@ -57750,7 +57747,7 @@
         <v>78</v>
       </c>
       <c r="F149" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G149" t="s">
         <v>54</v>
@@ -57822,7 +57819,7 @@
         <v>78</v>
       </c>
       <c r="F150" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G150" t="s">
         <v>7</v>
@@ -57845,7 +57842,7 @@
         <v>78</v>
       </c>
       <c r="F151" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G151" t="s">
         <v>62</v>
@@ -57914,7 +57911,7 @@
         <v>78</v>
       </c>
       <c r="F152" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G152" t="s">
         <v>64</v>
@@ -57983,7 +57980,7 @@
         <v>78</v>
       </c>
       <c r="F153" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G153" t="s">
         <v>65</v>
@@ -58052,7 +58049,7 @@
         <v>78</v>
       </c>
       <c r="F154" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G154" t="s">
         <v>67</v>
@@ -58081,7 +58078,7 @@
         <v>78</v>
       </c>
       <c r="F155" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G155" t="s">
         <v>68</v>
@@ -58150,7 +58147,7 @@
         <v>78</v>
       </c>
       <c r="F156" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G156" t="s">
         <v>69</v>
@@ -58219,7 +58216,7 @@
         <v>78</v>
       </c>
       <c r="F157" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G157" t="s">
         <v>71</v>
@@ -58288,7 +58285,7 @@
         <v>78</v>
       </c>
       <c r="F158" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G158" t="s">
         <v>54</v>
@@ -58360,7 +58357,7 @@
         <v>78</v>
       </c>
       <c r="F159" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G159" t="s">
         <v>54</v>
@@ -58432,7 +58429,7 @@
         <v>78</v>
       </c>
       <c r="F160" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G160" t="s">
         <v>7</v>
@@ -58455,7 +58452,7 @@
         <v>78</v>
       </c>
       <c r="F161" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G161" t="s">
         <v>62</v>
@@ -58524,7 +58521,7 @@
         <v>78</v>
       </c>
       <c r="F162" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G162" t="s">
         <v>64</v>
@@ -58593,7 +58590,7 @@
         <v>78</v>
       </c>
       <c r="F163" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G163" t="s">
         <v>65</v>
@@ -58662,7 +58659,7 @@
         <v>78</v>
       </c>
       <c r="F164" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G164" t="s">
         <v>67</v>
@@ -58691,7 +58688,7 @@
         <v>78</v>
       </c>
       <c r="F165" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G165" t="s">
         <v>68</v>
@@ -58760,7 +58757,7 @@
         <v>78</v>
       </c>
       <c r="F166" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G166" t="s">
         <v>69</v>
@@ -58829,7 +58826,7 @@
         <v>78</v>
       </c>
       <c r="F167" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G167" t="s">
         <v>71</v>
@@ -58898,7 +58895,7 @@
         <v>78</v>
       </c>
       <c r="F168" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G168" t="s">
         <v>54</v>
@@ -58970,7 +58967,7 @@
         <v>78</v>
       </c>
       <c r="F169" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G169" t="s">
         <v>54</v>
@@ -59042,13 +59039,13 @@
         <v>78</v>
       </c>
       <c r="F170" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G170" t="s">
         <v>54</v>
       </c>
       <c r="J170" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L170" t="s">
         <v>70</v>
@@ -59099,7 +59096,7 @@
     </row>
     <row r="171" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B171" t="s">
         <v>6</v>
@@ -59111,7 +59108,7 @@
         <v>17</v>
       </c>
       <c r="E171" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G171" t="s">
         <v>18</v>
@@ -59122,7 +59119,7 @@
     </row>
     <row r="172" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B172" t="s">
         <v>6</v>
@@ -59134,18 +59131,18 @@
         <v>17</v>
       </c>
       <c r="E172" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G172" t="s">
         <v>20</v>
       </c>
       <c r="H172" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="173" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B173" t="s">
         <v>6</v>
@@ -59157,16 +59154,16 @@
         <v>17</v>
       </c>
       <c r="E173" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G173" t="s">
         <v>54</v>
       </c>
       <c r="J173" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K173" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L173" t="s">
         <v>47</v>
@@ -59217,7 +59214,7 @@
     </row>
     <row r="174" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B174" t="s">
         <v>6</v>
@@ -59229,16 +59226,16 @@
         <v>17</v>
       </c>
       <c r="E174" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G174" t="s">
         <v>54</v>
       </c>
       <c r="J174" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K174" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L174" t="s">
         <v>47</v>
@@ -59289,7 +59286,7 @@
     </row>
     <row r="175" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B175" t="s">
         <v>6</v>
@@ -59301,7 +59298,7 @@
         <v>17</v>
       </c>
       <c r="E175" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G175" t="s">
         <v>18</v>
@@ -59312,7 +59309,7 @@
     </row>
     <row r="176" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B176" t="s">
         <v>6</v>
@@ -59324,7 +59321,7 @@
         <v>17</v>
       </c>
       <c r="E176" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G176" t="s">
         <v>20</v>
@@ -59335,7 +59332,7 @@
     </row>
     <row r="177" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B177" t="s">
         <v>6</v>
@@ -59347,13 +59344,13 @@
         <v>17</v>
       </c>
       <c r="E177" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G177" t="s">
         <v>58</v>
       </c>
       <c r="K177" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L177" t="s">
         <v>59</v>
@@ -59404,7 +59401,7 @@
     </row>
     <row r="178" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B178" t="s">
         <v>6</v>
@@ -59416,7 +59413,7 @@
         <v>17</v>
       </c>
       <c r="E178" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G178" t="s">
         <v>60</v>
@@ -59467,7 +59464,7 @@
     </row>
     <row r="179" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B179" t="s">
         <v>6</v>
@@ -59479,10 +59476,10 @@
         <v>17</v>
       </c>
       <c r="E179" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F179" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G179" t="s">
         <v>7</v>
@@ -59490,7 +59487,7 @@
     </row>
     <row r="180" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B180" t="s">
         <v>6</v>
@@ -59502,16 +59499,16 @@
         <v>17</v>
       </c>
       <c r="E180" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F180" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G180" t="s">
         <v>62</v>
       </c>
       <c r="K180" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L180" t="s">
         <v>63</v>
@@ -59562,7 +59559,7 @@
     </row>
     <row r="181" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B181" t="s">
         <v>6</v>
@@ -59574,16 +59571,16 @@
         <v>17</v>
       </c>
       <c r="E181" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F181" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G181" t="s">
         <v>64</v>
       </c>
       <c r="K181" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L181" t="s">
         <v>63</v>
@@ -59634,7 +59631,7 @@
     </row>
     <row r="182" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B182" t="s">
         <v>6</v>
@@ -59646,16 +59643,16 @@
         <v>17</v>
       </c>
       <c r="E182" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F182" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G182" t="s">
         <v>65</v>
       </c>
       <c r="K182" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L182" t="s">
         <v>66</v>
@@ -59706,7 +59703,7 @@
     </row>
     <row r="183" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B183" t="s">
         <v>6</v>
@@ -59718,16 +59715,16 @@
         <v>17</v>
       </c>
       <c r="E183" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F183" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G183" t="s">
         <v>67</v>
       </c>
       <c r="K183" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L183" t="s">
         <v>59</v>
@@ -59738,7 +59735,7 @@
     </row>
     <row r="184" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B184" t="s">
         <v>6</v>
@@ -59750,16 +59747,16 @@
         <v>17</v>
       </c>
       <c r="E184" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F184" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G184" t="s">
         <v>68</v>
       </c>
       <c r="K184" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L184" t="s">
         <v>47</v>
@@ -59810,7 +59807,7 @@
     </row>
     <row r="185" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B185" t="s">
         <v>6</v>
@@ -59822,16 +59819,16 @@
         <v>17</v>
       </c>
       <c r="E185" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F185" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G185" t="s">
         <v>69</v>
       </c>
       <c r="K185" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L185" t="s">
         <v>70</v>
@@ -59882,7 +59879,7 @@
     </row>
     <row r="186" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B186" t="s">
         <v>6</v>
@@ -59894,16 +59891,16 @@
         <v>17</v>
       </c>
       <c r="E186" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F186" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G186" t="s">
         <v>71</v>
       </c>
       <c r="K186" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L186" t="s">
         <v>70</v>
@@ -59954,7 +59951,7 @@
     </row>
     <row r="187" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B187" t="s">
         <v>6</v>
@@ -59966,10 +59963,10 @@
         <v>17</v>
       </c>
       <c r="E187" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F187" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G187" t="s">
         <v>54</v>
@@ -59978,7 +59975,7 @@
         <v>26</v>
       </c>
       <c r="K187" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L187" t="s">
         <v>19</v>
@@ -60029,7 +60026,7 @@
     </row>
     <row r="188" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B188" t="s">
         <v>6</v>
@@ -60041,19 +60038,19 @@
         <v>17</v>
       </c>
       <c r="E188" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F188" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G188" t="s">
         <v>54</v>
       </c>
       <c r="J188" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K188" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L188" t="s">
         <v>70</v>
@@ -60104,7 +60101,7 @@
     </row>
     <row r="189" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B189" t="s">
         <v>6</v>
@@ -60116,13 +60113,13 @@
         <v>17</v>
       </c>
       <c r="E189" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F189" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G189" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H189" t="s">
         <v>45</v>
@@ -60131,7 +60128,7 @@
         <v>46</v>
       </c>
       <c r="K189" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L189" t="s">
         <v>59</v>
@@ -60182,7 +60179,7 @@
     </row>
     <row r="190" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B190" t="s">
         <v>6</v>
@@ -60194,7 +60191,7 @@
         <v>17</v>
       </c>
       <c r="E190" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G190" t="s">
         <v>18</v>
@@ -60205,7 +60202,7 @@
     </row>
     <row r="191" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B191" t="s">
         <v>6</v>
@@ -60217,7 +60214,7 @@
         <v>17</v>
       </c>
       <c r="E191" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G191" t="s">
         <v>20</v>
@@ -60228,7 +60225,7 @@
     </row>
     <row r="192" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B192" t="s">
         <v>6</v>
@@ -60240,13 +60237,13 @@
         <v>17</v>
       </c>
       <c r="E192" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G192" t="s">
         <v>58</v>
       </c>
       <c r="K192" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L192" t="s">
         <v>59</v>
@@ -60297,7 +60294,7 @@
     </row>
     <row r="193" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B193" t="s">
         <v>6</v>
@@ -60309,7 +60306,7 @@
         <v>17</v>
       </c>
       <c r="E193" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G193" t="s">
         <v>60</v>
@@ -60360,7 +60357,7 @@
     </row>
     <row r="194" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B194" t="s">
         <v>6</v>
@@ -60372,10 +60369,10 @@
         <v>17</v>
       </c>
       <c r="E194" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F194" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G194" t="s">
         <v>7</v>
@@ -60383,7 +60380,7 @@
     </row>
     <row r="195" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B195" t="s">
         <v>6</v>
@@ -60395,16 +60392,16 @@
         <v>17</v>
       </c>
       <c r="E195" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F195" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G195" t="s">
         <v>62</v>
       </c>
       <c r="K195" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L195" t="s">
         <v>63</v>
@@ -60455,7 +60452,7 @@
     </row>
     <row r="196" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B196" t="s">
         <v>6</v>
@@ -60467,16 +60464,16 @@
         <v>17</v>
       </c>
       <c r="E196" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F196" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G196" t="s">
         <v>64</v>
       </c>
       <c r="K196" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L196" t="s">
         <v>63</v>
@@ -60527,7 +60524,7 @@
     </row>
     <row r="197" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B197" t="s">
         <v>6</v>
@@ -60539,16 +60536,16 @@
         <v>17</v>
       </c>
       <c r="E197" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F197" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G197" t="s">
         <v>65</v>
       </c>
       <c r="K197" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L197" t="s">
         <v>66</v>
@@ -60599,7 +60596,7 @@
     </row>
     <row r="198" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B198" t="s">
         <v>6</v>
@@ -60611,16 +60608,16 @@
         <v>17</v>
       </c>
       <c r="E198" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F198" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G198" t="s">
         <v>67</v>
       </c>
       <c r="K198" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L198" t="s">
         <v>59</v>
@@ -60631,7 +60628,7 @@
     </row>
     <row r="199" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B199" t="s">
         <v>6</v>
@@ -60643,16 +60640,16 @@
         <v>17</v>
       </c>
       <c r="E199" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F199" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G199" t="s">
         <v>68</v>
       </c>
       <c r="K199" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L199" t="s">
         <v>47</v>
@@ -60703,7 +60700,7 @@
     </row>
     <row r="200" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B200" t="s">
         <v>6</v>
@@ -60715,16 +60712,16 @@
         <v>17</v>
       </c>
       <c r="E200" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F200" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G200" t="s">
         <v>69</v>
       </c>
       <c r="K200" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L200" t="s">
         <v>70</v>
@@ -60775,7 +60772,7 @@
     </row>
     <row r="201" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B201" t="s">
         <v>6</v>
@@ -60787,16 +60784,16 @@
         <v>17</v>
       </c>
       <c r="E201" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F201" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G201" t="s">
         <v>71</v>
       </c>
       <c r="K201" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L201" t="s">
         <v>70</v>
@@ -60847,7 +60844,7 @@
     </row>
     <row r="202" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B202" t="s">
         <v>6</v>
@@ -60859,10 +60856,10 @@
         <v>17</v>
       </c>
       <c r="E202" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F202" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G202" t="s">
         <v>54</v>
@@ -60871,7 +60868,7 @@
         <v>37</v>
       </c>
       <c r="K202" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L202" t="s">
         <v>19</v>
@@ -60922,7 +60919,7 @@
     </row>
     <row r="203" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B203" t="s">
         <v>6</v>
@@ -60934,19 +60931,19 @@
         <v>17</v>
       </c>
       <c r="E203" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F203" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G203" t="s">
         <v>54</v>
       </c>
       <c r="J203" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K203" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L203" t="s">
         <v>70</v>
@@ -60997,7 +60994,7 @@
     </row>
     <row r="204" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B204" t="s">
         <v>6</v>
@@ -61009,13 +61006,13 @@
         <v>17</v>
       </c>
       <c r="E204" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F204" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G204" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H204" t="s">
         <v>45</v>
@@ -61024,7 +61021,7 @@
         <v>46</v>
       </c>
       <c r="K204" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L204" t="s">
         <v>59</v>

</xml_diff>